<commit_message>
Price coding and importing the product ingredients
4 hours
</commit_message>
<xml_diff>
--- a/documentation/Mixes.xlsx
+++ b/documentation/Mixes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="53">
   <si>
     <t>Grain</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>Unimix</t>
-  </si>
-  <si>
-    <t>%</t>
   </si>
   <si>
     <t>Cost</t>
@@ -196,10 +193,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -256,7 +252,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -267,12 +263,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency 2" xfId="3"/>
@@ -893,7 +885,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,6 +1060,9 @@
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="B16">
+        <v>2040</v>
+      </c>
       <c r="C16" s="4">
         <v>2701</v>
       </c>
@@ -1290,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="C179" sqref="C179"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,11 +1302,8 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>37</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1329,7 +1321,7 @@
         <v>300</v>
       </c>
       <c r="E2">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="F2">
         <v>90</v>
@@ -1350,7 +1342,7 @@
         <v>300</v>
       </c>
       <c r="E3">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="F3">
         <v>60</v>
@@ -1371,7 +1363,7 @@
         <v>260</v>
       </c>
       <c r="E4">
-        <v>0.19</v>
+        <v>19</v>
       </c>
       <c r="F4">
         <v>49.4</v>
@@ -1392,7 +1384,7 @@
         <v>250</v>
       </c>
       <c r="E5">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <v>37.5</v>
@@ -1413,7 +1405,7 @@
         <v>450</v>
       </c>
       <c r="E6">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="F6">
         <v>22.5</v>
@@ -1455,7 +1447,7 @@
         <v>275</v>
       </c>
       <c r="E8">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="F8">
         <v>16.5</v>
@@ -1476,7 +1468,7 @@
         <v>53</v>
       </c>
       <c r="E9">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="F9">
         <v>1.06</v>
@@ -1497,7 +1489,7 @@
         <v>226</v>
       </c>
       <c r="E10">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>2.2600000000000002</v>
@@ -1518,7 +1510,7 @@
         <v>264</v>
       </c>
       <c r="E11">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>2.64</v>
@@ -1539,7 +1531,7 @@
         <v>575</v>
       </c>
       <c r="E12">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>5.75</v>
@@ -1547,7 +1539,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14">
         <f>VLOOKUP(C14, 'Base Products'!A:C,2,FALSE)</f>
@@ -1560,17 +1552,17 @@
         <f>VLOOKUP(C14,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E14" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="F14" s="9">
-        <f t="shared" ref="F14:F24" si="0">+D14*E14</f>
-        <v>90</v>
+      <c r="E14">
+        <v>30</v>
+      </c>
+      <c r="F14" s="8" t="e">
+        <f>+D14*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15">
         <f>VLOOKUP(C15, 'Base Products'!A:C,2,FALSE)</f>
@@ -1583,17 +1575,17 @@
         <f>VLOOKUP(C15,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E15" s="8">
-        <v>0.23</v>
-      </c>
-      <c r="F15" s="9">
-        <f t="shared" si="0"/>
-        <v>69</v>
+      <c r="E15">
+        <v>23</v>
+      </c>
+      <c r="F15" s="8" t="e">
+        <f>+D15*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16">
         <f>VLOOKUP(C16, 'Base Products'!A:C,2,FALSE)</f>
@@ -1606,17 +1598,17 @@
         <f>VLOOKUP(C16,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>260</v>
       </c>
-      <c r="E16" s="8">
-        <v>0.21</v>
-      </c>
-      <c r="F16" s="9">
-        <f t="shared" si="0"/>
-        <v>54.6</v>
+      <c r="E16">
+        <v>21</v>
+      </c>
+      <c r="F16" s="8" t="e">
+        <f>+D16*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17">
         <f>VLOOKUP(C17, 'Base Products'!A:C,2,FALSE)</f>
@@ -1629,17 +1621,17 @@
         <f>VLOOKUP(C17,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>250</v>
       </c>
-      <c r="E17" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F17" s="9">
-        <f t="shared" si="0"/>
-        <v>25</v>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17" s="8" t="e">
+        <f>+D17*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18">
         <f>VLOOKUP(C18, 'Base Products'!A:C,2,FALSE)</f>
@@ -1652,17 +1644,17 @@
         <f>VLOOKUP(C18,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>450</v>
       </c>
-      <c r="E18" s="8">
-        <v>0.06</v>
-      </c>
-      <c r="F18" s="9">
-        <f t="shared" si="0"/>
-        <v>27</v>
+      <c r="E18">
+        <v>6</v>
+      </c>
+      <c r="F18" s="8" t="e">
+        <f>+D18*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19">
         <f>VLOOKUP(C19, 'Base Products'!A:C,2,FALSE)</f>
@@ -1675,17 +1667,17 @@
         <f>VLOOKUP(C19,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F19" s="8" t="e">
+        <f>+D19*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20">
         <f>VLOOKUP(C20, 'Base Products'!A:C,2,FALSE)</f>
@@ -1698,17 +1690,17 @@
         <f>VLOOKUP(C20,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>275</v>
       </c>
-      <c r="E20" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="F20" s="9">
-        <f t="shared" si="0"/>
-        <v>13.75</v>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20" s="8" t="e">
+        <f>+D20*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <f>VLOOKUP(C21, 'Base Products'!A:C,2,FALSE)</f>
@@ -1721,17 +1713,17 @@
         <f>VLOOKUP(C21,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>53</v>
       </c>
-      <c r="E21" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F21" s="9">
-        <f t="shared" si="0"/>
-        <v>1.06</v>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21" s="8" t="e">
+        <f>+D21*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <f>VLOOKUP(C22, 'Base Products'!A:C,2,FALSE)</f>
@@ -1744,17 +1736,17 @@
         <f>VLOOKUP(C22,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>226</v>
       </c>
-      <c r="E22" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F22" s="9">
-        <f t="shared" si="0"/>
-        <v>2.2600000000000002</v>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="8" t="e">
+        <f>+D22*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23">
         <f>VLOOKUP(C23, 'Base Products'!A:C,2,FALSE)</f>
@@ -1767,17 +1759,17 @@
         <f>VLOOKUP(C23,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>264</v>
       </c>
-      <c r="E23" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F23" s="9">
-        <f t="shared" si="0"/>
-        <v>2.64</v>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="8" t="e">
+        <f>+D23*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <f>VLOOKUP(C24, 'Base Products'!A:C,2,FALSE)</f>
@@ -1790,23 +1782,22 @@
         <f>VLOOKUP(C24,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>575</v>
       </c>
-      <c r="E24" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F24" s="9">
-        <f t="shared" si="0"/>
-        <v>5.75</v>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" s="8" t="e">
+        <f>+D24*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="9"/>
+      <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26">
         <f>VLOOKUP(C26, 'Base Products'!A:C,2,FALSE)</f>
@@ -1819,17 +1810,17 @@
         <f>VLOOKUP(C26,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E26" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="F26" s="9">
-        <f t="shared" ref="F26:F37" si="1">+D26*E26</f>
-        <v>90</v>
+      <c r="E26">
+        <v>30</v>
+      </c>
+      <c r="F26" s="8" t="e">
+        <f>+D26*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27">
         <f>VLOOKUP(C27, 'Base Products'!A:C,2,FALSE)</f>
@@ -1842,17 +1833,17 @@
         <f>VLOOKUP(C27,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E27" s="8">
-        <v>0.22</v>
-      </c>
-      <c r="F27" s="9">
-        <f t="shared" si="1"/>
-        <v>66</v>
+      <c r="E27">
+        <v>22</v>
+      </c>
+      <c r="F27" s="8" t="e">
+        <f>+D27*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28">
         <f>VLOOKUP(C28, 'Base Products'!A:C,2,FALSE)</f>
@@ -1865,17 +1856,17 @@
         <f>VLOOKUP(C28,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>260</v>
       </c>
-      <c r="E28" s="8">
-        <v>0.13</v>
-      </c>
-      <c r="F28" s="9">
-        <f t="shared" si="1"/>
-        <v>33.800000000000004</v>
+      <c r="E28">
+        <v>13</v>
+      </c>
+      <c r="F28" s="8" t="e">
+        <f>+D28*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29">
         <f>VLOOKUP(C29, 'Base Products'!A:C,2,FALSE)</f>
@@ -1888,17 +1879,17 @@
         <f>VLOOKUP(C29,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>450</v>
       </c>
-      <c r="E29" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F29" s="9">
-        <f t="shared" si="1"/>
-        <v>45</v>
+      <c r="E29">
+        <v>10</v>
+      </c>
+      <c r="F29" s="8" t="e">
+        <f>+D29*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30">
         <f>VLOOKUP(C30, 'Base Products'!A:C,2,FALSE)</f>
@@ -1911,17 +1902,17 @@
         <f>VLOOKUP(C30,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>250</v>
       </c>
-      <c r="E30" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F30" s="9">
-        <f t="shared" si="1"/>
-        <v>25</v>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30" s="8" t="e">
+        <f>+D30*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31">
         <f>VLOOKUP(C31, 'Base Products'!A:C,2,FALSE)</f>
@@ -1934,17 +1925,17 @@
         <f>VLOOKUP(C31,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>430</v>
       </c>
-      <c r="E31" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="F31" s="9">
-        <f t="shared" si="1"/>
-        <v>21.5</v>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31" s="8" t="e">
+        <f>+D31*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32">
         <f>VLOOKUP(C32, 'Base Products'!A:C,2,FALSE)</f>
@@ -1957,17 +1948,17 @@
         <f>VLOOKUP(C32,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>275</v>
       </c>
-      <c r="E32" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="F32" s="9">
-        <f t="shared" si="1"/>
-        <v>13.75</v>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32" s="8" t="e">
+        <f>+D32*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33">
         <f>VLOOKUP(C33, 'Base Products'!A:C,2,FALSE)</f>
@@ -1980,17 +1971,17 @@
         <f>VLOOKUP(C33,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33">
         <v>0</v>
       </c>
-      <c r="F33" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F33" s="8" t="e">
+        <f>+D33*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34">
         <f>VLOOKUP(C34, 'Base Products'!A:C,2,FALSE)</f>
@@ -2003,17 +1994,17 @@
         <f>VLOOKUP(C34,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>53</v>
       </c>
-      <c r="E34" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F34" s="9">
-        <f t="shared" si="1"/>
-        <v>1.06</v>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34" s="8" t="e">
+        <f>+D34*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35">
         <f>VLOOKUP(C35, 'Base Products'!A:C,2,FALSE)</f>
@@ -2026,17 +2017,17 @@
         <f>VLOOKUP(C35,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>226</v>
       </c>
-      <c r="E35" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F35" s="9">
-        <f t="shared" si="1"/>
-        <v>2.2600000000000002</v>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" s="8" t="e">
+        <f>+D35*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36">
         <f>VLOOKUP(C36, 'Base Products'!A:C,2,FALSE)</f>
@@ -2049,17 +2040,17 @@
         <f>VLOOKUP(C36,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>264</v>
       </c>
-      <c r="E36" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F36" s="9">
-        <f t="shared" si="1"/>
-        <v>2.64</v>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" s="8" t="e">
+        <f>+D36*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37">
         <f>VLOOKUP(C37, 'Base Products'!A:C,2,FALSE)</f>
@@ -2072,17 +2063,17 @@
         <f>VLOOKUP(C37,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>575</v>
       </c>
-      <c r="E37" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F37" s="9">
-        <f t="shared" si="1"/>
-        <v>5.75</v>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" s="8" t="e">
+        <f>+D37*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39">
         <f>VLOOKUP(C39, 'Base Products'!A:C,2,FALSE)</f>
@@ -2095,17 +2086,17 @@
         <f>VLOOKUP(C39,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E39" s="8">
-        <v>0.25</v>
-      </c>
-      <c r="F39" s="9">
-        <f t="shared" ref="F39:F50" si="2">+D39*E39</f>
-        <v>75</v>
+      <c r="E39">
+        <v>25</v>
+      </c>
+      <c r="F39" s="8" t="e">
+        <f>+D39*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40">
         <f>VLOOKUP(C40, 'Base Products'!A:C,2,FALSE)</f>
@@ -2118,17 +2109,17 @@
         <f>VLOOKUP(C40,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E40" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="F40" s="9">
-        <f t="shared" si="2"/>
-        <v>60</v>
+      <c r="E40">
+        <v>20</v>
+      </c>
+      <c r="F40" s="8" t="e">
+        <f>+D40*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41">
         <f>VLOOKUP(C41, 'Base Products'!A:C,2,FALSE)</f>
@@ -2141,86 +2132,86 @@
         <f>VLOOKUP(C41,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>450</v>
       </c>
-      <c r="E41" s="8">
-        <v>0.18</v>
-      </c>
-      <c r="F41" s="9">
-        <f t="shared" si="2"/>
-        <v>81</v>
+      <c r="E41">
+        <v>18</v>
+      </c>
+      <c r="F41" s="8" t="e">
+        <f>+D41*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <f>VLOOKUP(C42, 'Base Products'!A:C,2,FALSE)</f>
         <v>2002</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D42" s="5">
         <f>VLOOKUP(C42,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>260</v>
       </c>
-      <c r="E42" s="12">
-        <v>0.13</v>
-      </c>
-      <c r="F42" s="9">
-        <f t="shared" si="2"/>
-        <v>33.800000000000004</v>
+      <c r="E42">
+        <v>13</v>
+      </c>
+      <c r="F42" s="8" t="e">
+        <f>+D42*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43">
         <f>VLOOKUP(C43, 'Base Products'!A:C,2,FALSE)</f>
         <v>2013</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="5">
         <f>VLOOKUP(C43,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>250</v>
       </c>
-      <c r="E43" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="F43" s="9">
-        <f t="shared" si="2"/>
-        <v>25</v>
+      <c r="E43">
+        <v>10</v>
+      </c>
+      <c r="F43" s="8" t="e">
+        <f>+D43*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44">
         <f>VLOOKUP(C44, 'Base Products'!A:C,2,FALSE)</f>
         <v>2014</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="5">
         <f>VLOOKUP(C44,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E44" s="12">
+      <c r="E44">
         <v>0</v>
       </c>
-      <c r="F44" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="F44" s="8" t="e">
+        <f>+D44*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45">
         <f>VLOOKUP(C45, 'Base Products'!A:C,2,FALSE)</f>
@@ -2233,132 +2224,132 @@
         <f>VLOOKUP(C45,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>275</v>
       </c>
-      <c r="E45" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="F45" s="9">
-        <f t="shared" si="2"/>
-        <v>13.75</v>
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45" s="8" t="e">
+        <f>+D45*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46">
         <f>VLOOKUP(C46, 'Base Products'!A:C,2,FALSE)</f>
         <v>2009</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D46" s="5">
         <f>VLOOKUP(C46,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>430</v>
       </c>
-      <c r="E46" s="12">
-        <v>0.04</v>
-      </c>
-      <c r="F46" s="9">
-        <f t="shared" si="2"/>
-        <v>17.2</v>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46" s="8" t="e">
+        <f>+D46*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47">
         <f>VLOOKUP(C47, 'Base Products'!A:C,2,FALSE)</f>
         <v>2024</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="5">
         <f>VLOOKUP(C47,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>53</v>
       </c>
-      <c r="E47" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="F47" s="9">
-        <f t="shared" si="2"/>
-        <v>1.06</v>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" s="8" t="e">
+        <f>+D47*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48">
         <f>VLOOKUP(C48, 'Base Products'!A:C,2,FALSE)</f>
         <v>2025</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="5">
         <f>VLOOKUP(C48,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>226</v>
       </c>
-      <c r="E48" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="F48" s="9">
-        <f t="shared" si="2"/>
-        <v>2.2600000000000002</v>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="8" t="e">
+        <f>+D48*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49">
         <f>VLOOKUP(C49, 'Base Products'!A:C,2,FALSE)</f>
         <v>4031</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="5">
         <f>VLOOKUP(C49,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>264</v>
       </c>
-      <c r="E49" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="F49" s="9">
-        <f t="shared" si="2"/>
-        <v>2.64</v>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="8" t="e">
+        <f>+D49*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50">
         <f>VLOOKUP(C50, 'Base Products'!A:C,2,FALSE)</f>
         <v>4034</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="9" t="s">
         <v>34</v>
       </c>
       <c r="D50" s="5">
         <f>VLOOKUP(C50,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>575</v>
       </c>
-      <c r="E50" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="F50" s="9">
-        <f t="shared" si="2"/>
-        <v>5.75</v>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="8" t="e">
+        <f>+D50*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B52">
         <f>VLOOKUP(C52, 'Base Products'!A:C,2,FALSE)</f>
@@ -2371,17 +2362,17 @@
         <f>VLOOKUP(C52,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>450</v>
       </c>
-      <c r="E52" s="8">
-        <v>0.22</v>
-      </c>
-      <c r="F52" s="9">
-        <f t="shared" ref="F52:F63" si="3">+D52*E52</f>
-        <v>99</v>
+      <c r="E52">
+        <v>22</v>
+      </c>
+      <c r="F52" s="8" t="e">
+        <f>+D52*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B53">
         <f>VLOOKUP(C53, 'Base Products'!A:C,2,FALSE)</f>
@@ -2394,17 +2385,17 @@
         <f>VLOOKUP(C53,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E53" s="8">
-        <v>0.18</v>
-      </c>
-      <c r="F53" s="9">
-        <f t="shared" si="3"/>
-        <v>54</v>
+      <c r="E53">
+        <v>18</v>
+      </c>
+      <c r="F53" s="8" t="e">
+        <f>+D53*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B54">
         <f>VLOOKUP(C54, 'Base Products'!A:C,2,FALSE)</f>
@@ -2417,17 +2408,17 @@
         <f>VLOOKUP(C54,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E54" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="F54" s="9">
-        <f t="shared" si="3"/>
-        <v>45</v>
+      <c r="E54">
+        <v>15</v>
+      </c>
+      <c r="F54" s="8" t="e">
+        <f>+D54*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B55">
         <f>VLOOKUP(C55, 'Base Products'!A:C,2,FALSE)</f>
@@ -2440,17 +2431,17 @@
         <f>VLOOKUP(C55,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>260</v>
       </c>
-      <c r="E55" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="F55" s="9">
-        <f t="shared" si="3"/>
-        <v>39</v>
+      <c r="E55">
+        <v>15</v>
+      </c>
+      <c r="F55" s="8" t="e">
+        <f>+D55*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B56">
         <f>VLOOKUP(C56, 'Base Products'!A:C,2,FALSE)</f>
@@ -2463,17 +2454,17 @@
         <f>VLOOKUP(C56,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>250</v>
       </c>
-      <c r="E56" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F56" s="9">
-        <f t="shared" si="3"/>
-        <v>25</v>
+      <c r="E56">
+        <v>10</v>
+      </c>
+      <c r="F56" s="8" t="e">
+        <f>+D56*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B57">
         <f>VLOOKUP(C57, 'Base Products'!A:C,2,FALSE)</f>
@@ -2486,17 +2477,17 @@
         <f>VLOOKUP(C57,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>430</v>
       </c>
-      <c r="E57" s="8">
-        <v>0.08</v>
-      </c>
-      <c r="F57" s="9">
-        <f t="shared" si="3"/>
-        <v>34.4</v>
+      <c r="E57">
+        <v>8</v>
+      </c>
+      <c r="F57" s="8" t="e">
+        <f>+D57*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B58">
         <f>VLOOKUP(C58, 'Base Products'!A:C,2,FALSE)</f>
@@ -2509,17 +2500,17 @@
         <f>VLOOKUP(C58,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>275</v>
       </c>
-      <c r="E58" s="8">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F58" s="9">
-        <f t="shared" si="3"/>
-        <v>19.250000000000004</v>
+      <c r="E58">
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="F58" s="8" t="e">
+        <f>+D58*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B59">
         <f>VLOOKUP(C59, 'Base Products'!A:C,2,FALSE)</f>
@@ -2532,17 +2523,17 @@
         <f>VLOOKUP(C59,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E59" s="8">
+      <c r="E59">
         <v>0</v>
       </c>
-      <c r="F59" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="F59" s="8" t="e">
+        <f>+D59*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B60">
         <f>VLOOKUP(C60, 'Base Products'!A:C,2,FALSE)</f>
@@ -2555,17 +2546,17 @@
         <f>VLOOKUP(C60,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>53</v>
       </c>
-      <c r="E60" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F60" s="9">
-        <f t="shared" si="3"/>
-        <v>1.06</v>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60" s="8" t="e">
+        <f>+D60*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B61">
         <f>VLOOKUP(C61, 'Base Products'!A:C,2,FALSE)</f>
@@ -2578,17 +2569,17 @@
         <f>VLOOKUP(C61,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>226</v>
       </c>
-      <c r="E61" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F61" s="9">
-        <f t="shared" si="3"/>
-        <v>2.2600000000000002</v>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" s="8" t="e">
+        <f>+D61*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B62">
         <f>VLOOKUP(C62, 'Base Products'!A:C,2,FALSE)</f>
@@ -2601,17 +2592,17 @@
         <f>VLOOKUP(C62,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>264</v>
       </c>
-      <c r="E62" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F62" s="9">
-        <f t="shared" si="3"/>
-        <v>2.64</v>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" s="8" t="e">
+        <f>+D62*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B63">
         <f>VLOOKUP(C63, 'Base Products'!A:C,2,FALSE)</f>
@@ -2624,17 +2615,17 @@
         <f>VLOOKUP(C63,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>575</v>
       </c>
-      <c r="E63" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F63" s="9">
-        <f t="shared" si="3"/>
-        <v>5.75</v>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63" s="8" t="e">
+        <f>+D63*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B65">
         <f>VLOOKUP(C65, 'Base Products'!A:C,2,FALSE)</f>
@@ -2647,17 +2638,17 @@
         <f>VLOOKUP(C65,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E65" s="8">
-        <v>0.35</v>
-      </c>
-      <c r="F65" s="9">
-        <f t="shared" ref="F65:F75" si="4">+D65*E65</f>
-        <v>105</v>
+      <c r="E65">
+        <v>35</v>
+      </c>
+      <c r="F65" s="8" t="e">
+        <f>+D65*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B66">
         <f>VLOOKUP(C66, 'Base Products'!A:C,2,FALSE)</f>
@@ -2670,17 +2661,17 @@
         <f>VLOOKUP(C66,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E66" s="8">
-        <v>0.25</v>
-      </c>
-      <c r="F66" s="9">
-        <f t="shared" si="4"/>
-        <v>75</v>
+      <c r="E66">
+        <v>25</v>
+      </c>
+      <c r="F66" s="8" t="e">
+        <f>+D66*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B67">
         <f>VLOOKUP(C67, 'Base Products'!A:C,2,FALSE)</f>
@@ -2693,17 +2684,17 @@
         <f>VLOOKUP(C67,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>260</v>
       </c>
-      <c r="E67" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F67" s="9">
-        <f t="shared" si="4"/>
-        <v>26</v>
+      <c r="E67">
+        <v>10</v>
+      </c>
+      <c r="F67" s="8" t="e">
+        <f>+D67*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B68">
         <f>VLOOKUP(C68, 'Base Products'!A:C,2,FALSE)</f>
@@ -2716,17 +2707,17 @@
         <f>VLOOKUP(C68,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>450</v>
       </c>
-      <c r="E68" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F68" s="9">
-        <f t="shared" si="4"/>
-        <v>45</v>
+      <c r="E68">
+        <v>10</v>
+      </c>
+      <c r="F68" s="8" t="e">
+        <f>+D68*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B69">
         <f>VLOOKUP(C69, 'Base Products'!A:C,2,FALSE)</f>
@@ -2739,17 +2730,17 @@
         <f>VLOOKUP(C69,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E69" s="8">
+      <c r="E69">
         <v>0</v>
       </c>
-      <c r="F69" s="9">
-        <f t="shared" si="4"/>
-        <v>0</v>
+      <c r="F69" s="8" t="e">
+        <f>+D69*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B70">
         <f>VLOOKUP(C70, 'Base Products'!A:C,2,FALSE)</f>
@@ -2762,17 +2753,17 @@
         <f>VLOOKUP(C70,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>275</v>
       </c>
-      <c r="E70" s="8">
-        <v>0.08</v>
-      </c>
-      <c r="F70" s="9">
-        <f t="shared" si="4"/>
-        <v>22</v>
+      <c r="E70">
+        <v>8</v>
+      </c>
+      <c r="F70" s="8" t="e">
+        <f>+D70*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B71">
         <f>VLOOKUP(C71, 'Base Products'!A:C,2,FALSE)</f>
@@ -2785,17 +2776,17 @@
         <f>VLOOKUP(C71,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>315</v>
       </c>
-      <c r="E71" s="8">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F71" s="9">
-        <f t="shared" si="4"/>
-        <v>22.05</v>
+      <c r="E71">
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="F71" s="8" t="e">
+        <f>+D71*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B72">
         <f>VLOOKUP(C72, 'Base Products'!A:C,2,FALSE)</f>
@@ -2808,17 +2799,17 @@
         <f>VLOOKUP(C72,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>53</v>
       </c>
-      <c r="E72" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F72" s="9">
-        <f t="shared" si="4"/>
-        <v>1.06</v>
+      <c r="E72">
+        <v>2</v>
+      </c>
+      <c r="F72" s="8" t="e">
+        <f>+D72*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B73">
         <f>VLOOKUP(C73, 'Base Products'!A:C,2,FALSE)</f>
@@ -2831,17 +2822,17 @@
         <f>VLOOKUP(C73,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>226</v>
       </c>
-      <c r="E73" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F73" s="9">
-        <f t="shared" si="4"/>
-        <v>2.2600000000000002</v>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73" s="8" t="e">
+        <f>+D73*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B74">
         <f>VLOOKUP(C74, 'Base Products'!A:C,2,FALSE)</f>
@@ -2854,17 +2845,17 @@
         <f>VLOOKUP(C74,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>264</v>
       </c>
-      <c r="E74" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F74" s="9">
-        <f t="shared" si="4"/>
-        <v>2.64</v>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74" s="8" t="e">
+        <f>+D74*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B75">
         <f>VLOOKUP(C75, 'Base Products'!A:C,2,FALSE)</f>
@@ -2877,17 +2868,17 @@
         <f>VLOOKUP(C75,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>575</v>
       </c>
-      <c r="E75" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F75" s="9">
-        <f t="shared" si="4"/>
-        <v>5.75</v>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75" s="8" t="e">
+        <f>+D75*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B77">
         <f>VLOOKUP(C77, 'Base Products'!A:C,2,FALSE)</f>
@@ -2900,17 +2891,17 @@
         <f>VLOOKUP(C77,[1]Prices!$A$1:$B$35,2,FALSE)</f>
         <v>260</v>
       </c>
-      <c r="E77" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F77" s="9">
-        <f t="shared" ref="F77:F90" si="5">+D77*E77</f>
-        <v>130</v>
+      <c r="E77">
+        <v>50</v>
+      </c>
+      <c r="F77" s="8" t="e">
+        <f>+D77*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B78">
         <f>VLOOKUP(C78, 'Base Products'!A:C,2,FALSE)</f>
@@ -2923,17 +2914,17 @@
         <f>VLOOKUP(C78,[1]Prices!$A$1:$B$35,2,FALSE)</f>
         <v>275</v>
       </c>
-      <c r="E78" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="F78" s="9">
-        <f t="shared" si="5"/>
-        <v>82.5</v>
+      <c r="E78">
+        <v>30</v>
+      </c>
+      <c r="F78" s="8" t="e">
+        <f>+D78*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B79">
         <f>VLOOKUP(C79, 'Base Products'!A:C,2,FALSE)</f>
@@ -2946,17 +2937,17 @@
         <f>VLOOKUP(C79,[1]Prices!$A$1:$B$35,2,FALSE)</f>
         <v>285</v>
       </c>
-      <c r="E79" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F79" s="9">
-        <f t="shared" si="5"/>
-        <v>28.5</v>
+      <c r="E79">
+        <v>10</v>
+      </c>
+      <c r="F79" s="8" t="e">
+        <f>+D79*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B80">
         <f>VLOOKUP(C80, 'Base Products'!A:C,2,FALSE)</f>
@@ -2969,17 +2960,17 @@
         <f>VLOOKUP(C80,[1]Prices!$A$1:$B$35,2,FALSE)</f>
         <v>127</v>
       </c>
-      <c r="E80" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F80" s="9">
-        <f t="shared" si="5"/>
-        <v>12.700000000000001</v>
+      <c r="E80">
+        <v>10</v>
+      </c>
+      <c r="F80" s="8" t="e">
+        <f>+D80*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B81">
         <f>VLOOKUP(C81, 'Base Products'!A:C,2,FALSE)</f>
@@ -2992,17 +2983,17 @@
         <f>VLOOKUP(C81,[1]Prices!$A$1:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E81" s="8">
+      <c r="E81">
         <v>0</v>
       </c>
-      <c r="F81" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
+      <c r="F81" s="8" t="e">
+        <f>+D81*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B82">
         <f>VLOOKUP(C82, 'Base Products'!A:C,2,FALSE)</f>
@@ -3015,17 +3006,17 @@
         <f>VLOOKUP(C82,[1]Prices!$A$1:$B$35,2,FALSE)</f>
         <v>250</v>
       </c>
-      <c r="E82" s="8">
+      <c r="E82">
         <v>0</v>
       </c>
-      <c r="F82" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
+      <c r="F82" s="8" t="e">
+        <f>+D82*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B83">
         <f>VLOOKUP(C83, 'Base Products'!A:C,2,FALSE)</f>
@@ -3038,17 +3029,17 @@
         <f>VLOOKUP(C83,[1]Prices!$A$1:$B$35,2,FALSE)</f>
         <v>450</v>
       </c>
-      <c r="E83" s="8">
+      <c r="E83">
         <v>0</v>
       </c>
-      <c r="F83" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
+      <c r="F83" s="8" t="e">
+        <f>+D83*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B84">
         <f>VLOOKUP(C84, 'Base Products'!A:C,2,FALSE)</f>
@@ -3061,17 +3052,17 @@
         <f>VLOOKUP(C84,[1]Prices!$A$1:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E84" s="8">
+      <c r="E84">
         <v>0</v>
       </c>
-      <c r="F84" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
+      <c r="F84" s="8" t="e">
+        <f>+D84*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B85">
         <f>VLOOKUP(C85, 'Base Products'!A:C,2,FALSE)</f>
@@ -3084,17 +3075,17 @@
         <f>VLOOKUP(C85,[1]Prices!$A$1:$B$35,2,FALSE)</f>
         <v>226</v>
       </c>
-      <c r="E85" s="8">
+      <c r="E85">
         <v>0</v>
       </c>
-      <c r="F85" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
+      <c r="F85" s="8" t="e">
+        <f>+D85*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B86">
         <f>VLOOKUP(C86, 'Base Products'!A:C,2,FALSE)</f>
@@ -3107,17 +3098,17 @@
         <f>VLOOKUP(C86,[1]Prices!$A$1:$B$35,2,FALSE)</f>
         <v>264</v>
       </c>
-      <c r="E86" s="8">
+      <c r="E86">
         <v>0</v>
       </c>
-      <c r="F86" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
+      <c r="F86" s="8" t="e">
+        <f>+D86*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B87">
         <f>VLOOKUP(C87, 'Base Products'!A:C,2,FALSE)</f>
@@ -3130,17 +3121,17 @@
         <f>VLOOKUP(C87,[1]Prices!$A$1:$B$35,2,FALSE)</f>
         <v>53</v>
       </c>
-      <c r="E87" s="8">
+      <c r="E87">
         <v>0</v>
       </c>
-      <c r="F87" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
+      <c r="F87" s="8" t="e">
+        <f>+D87*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B88">
         <f>VLOOKUP(C88, 'Base Products'!A:C,2,FALSE)</f>
@@ -3153,17 +3144,17 @@
         <f>VLOOKUP(C88,[1]Prices!$A$1:$B$35,2,FALSE)</f>
         <v>575</v>
       </c>
-      <c r="E88" s="8">
+      <c r="E88">
         <v>0</v>
       </c>
-      <c r="F88" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
+      <c r="F88" s="8" t="e">
+        <f>+D88*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B89">
         <f>VLOOKUP(C89, 'Base Products'!A:C,2,FALSE)</f>
@@ -3176,17 +3167,17 @@
         <f>VLOOKUP(C89,[1]Prices!$A$1:$B$35,2,FALSE)</f>
         <v>7865</v>
       </c>
-      <c r="E89" s="8">
+      <c r="E89">
         <v>0</v>
       </c>
-      <c r="F89" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
+      <c r="F89" s="8" t="e">
+        <f>+D89*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B90">
         <f>VLOOKUP(C90, 'Base Products'!A:C,2,FALSE)</f>
@@ -3199,17 +3190,17 @@
         <f>VLOOKUP(C90,[1]Prices!$A$1:$B$35,2,FALSE)</f>
         <v>7271</v>
       </c>
-      <c r="E90" s="8">
+      <c r="E90">
         <v>0</v>
       </c>
-      <c r="F90" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
+      <c r="F90" s="8" t="e">
+        <f>+D90*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B92">
         <f>VLOOKUP(C92, 'Base Products'!A:C,2,FALSE)</f>
@@ -3222,17 +3213,17 @@
         <f>VLOOKUP(C92,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E92" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="F92" s="9">
-        <f t="shared" ref="F92:F104" si="6">+D92*E92</f>
-        <v>60</v>
+      <c r="E92">
+        <v>20</v>
+      </c>
+      <c r="F92" s="8" t="e">
+        <f>+D92*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B93">
         <f>VLOOKUP(C93, 'Base Products'!A:C,2,FALSE)</f>
@@ -3245,17 +3236,17 @@
         <f>VLOOKUP(C93,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>450</v>
       </c>
-      <c r="E93" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="F93" s="9">
-        <f t="shared" si="6"/>
-        <v>90</v>
+      <c r="E93">
+        <v>20</v>
+      </c>
+      <c r="F93" s="8" t="e">
+        <f>+D93*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B94">
         <f>VLOOKUP(C94, 'Base Products'!A:C,2,FALSE)</f>
@@ -3268,17 +3259,17 @@
         <f>VLOOKUP(C94,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>260</v>
       </c>
-      <c r="E94" s="8">
-        <v>0.14749999999999999</v>
-      </c>
-      <c r="F94" s="9">
-        <f t="shared" si="6"/>
-        <v>38.35</v>
+      <c r="E94">
+        <v>14.75</v>
+      </c>
+      <c r="F94" s="8" t="e">
+        <f>+D94*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B95">
         <f>VLOOKUP(C95, 'Base Products'!A:C,2,FALSE)</f>
@@ -3291,17 +3282,17 @@
         <f>VLOOKUP(C95,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E95" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F95" s="9">
-        <f t="shared" si="6"/>
-        <v>30</v>
+      <c r="E95">
+        <v>10</v>
+      </c>
+      <c r="F95" s="8" t="e">
+        <f>+D95*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B96">
         <f>VLOOKUP(C96, 'Base Products'!A:C,2,FALSE)</f>
@@ -3314,17 +3305,17 @@
         <f>VLOOKUP(C96,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>315</v>
       </c>
-      <c r="E96" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F96" s="9">
-        <f t="shared" si="6"/>
-        <v>31.5</v>
+      <c r="E96">
+        <v>10</v>
+      </c>
+      <c r="F96" s="8" t="e">
+        <f>+D96*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B97">
         <f>VLOOKUP(C97, 'Base Products'!A:C,2,FALSE)</f>
@@ -3337,17 +3328,17 @@
         <f>VLOOKUP(C97,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>430</v>
       </c>
-      <c r="E97" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F97" s="9">
-        <f t="shared" si="6"/>
-        <v>43</v>
+      <c r="E97">
+        <v>10</v>
+      </c>
+      <c r="F97" s="8" t="e">
+        <f>+D97*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B98">
         <f>VLOOKUP(C98, 'Base Products'!A:C,2,FALSE)</f>
@@ -3360,17 +3351,17 @@
         <f>VLOOKUP(C98,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>250</v>
       </c>
-      <c r="E98" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F98" s="9">
-        <f t="shared" si="6"/>
-        <v>25</v>
+      <c r="E98">
+        <v>10</v>
+      </c>
+      <c r="F98" s="8" t="e">
+        <f>+D98*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B99">
         <f>VLOOKUP(C99, 'Base Products'!A:C,2,FALSE)</f>
@@ -3383,17 +3374,17 @@
         <f>VLOOKUP(C99,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>53</v>
       </c>
-      <c r="E99" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F99" s="9">
-        <f t="shared" si="6"/>
-        <v>1.06</v>
+      <c r="E99">
+        <v>2</v>
+      </c>
+      <c r="F99" s="8" t="e">
+        <f>+D99*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B100">
         <f>VLOOKUP(C100, 'Base Products'!A:C,2,FALSE)</f>
@@ -3406,17 +3397,17 @@
         <f>VLOOKUP(C100,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>594</v>
       </c>
-      <c r="E100" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F100" s="9">
-        <f t="shared" si="6"/>
-        <v>5.94</v>
+      <c r="E100">
+        <v>1</v>
+      </c>
+      <c r="F100" s="8" t="e">
+        <f>+D100*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B101">
         <f>VLOOKUP(C101, 'Base Products'!A:C,2,FALSE)</f>
@@ -3429,17 +3420,17 @@
         <f>VLOOKUP(C101,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>264</v>
       </c>
-      <c r="E101" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F101" s="9">
-        <f t="shared" si="6"/>
-        <v>2.64</v>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101" s="8" t="e">
+        <f>+D101*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B102">
         <f>VLOOKUP(C102, 'Base Products'!A:C,2,FALSE)</f>
@@ -3452,21 +3443,21 @@
         <f>VLOOKUP(C102,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>575</v>
       </c>
-      <c r="E102" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F102" s="9">
-        <f t="shared" si="6"/>
-        <v>5.75</v>
+      <c r="E102">
+        <v>1</v>
+      </c>
+      <c r="F102" s="8" t="e">
+        <f>+D102*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B103">
         <f>VLOOKUP(C103, 'Base Products'!A:C,2,FALSE)</f>
-        <v>0</v>
+        <v>2040</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>16</v>
@@ -3475,17 +3466,17 @@
         <f>VLOOKUP(C103,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>2701</v>
       </c>
-      <c r="E103" s="8">
-        <v>2E-3</v>
-      </c>
-      <c r="F103" s="9">
-        <f t="shared" si="6"/>
-        <v>5.4020000000000001</v>
+      <c r="E103">
+        <v>0.2</v>
+      </c>
+      <c r="F103" s="8" t="e">
+        <f>+D103*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B104">
         <f>VLOOKUP(C104, 'Base Products'!A:C,2,FALSE)</f>
@@ -3498,17 +3489,17 @@
         <f>VLOOKUP(C104,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>7271</v>
       </c>
-      <c r="E104" s="8">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="F104" s="9">
-        <f t="shared" si="6"/>
-        <v>3.6355</v>
+      <c r="E104">
+        <v>0.05</v>
+      </c>
+      <c r="F104" s="8" t="e">
+        <f>+D104*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B106">
         <f>VLOOKUP(C106, 'Base Products'!A:C,2,FALSE)</f>
@@ -3521,17 +3512,17 @@
         <f>VLOOKUP(C106,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>450</v>
       </c>
-      <c r="E106" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="F106" s="9">
-        <f t="shared" ref="F106:F119" si="7">+D106*E106</f>
-        <v>90</v>
+      <c r="E106">
+        <v>20</v>
+      </c>
+      <c r="F106" s="8" t="e">
+        <f>+D106*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B107">
         <f>VLOOKUP(C107, 'Base Products'!A:C,2,FALSE)</f>
@@ -3544,17 +3535,17 @@
         <f>VLOOKUP(C107,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>430</v>
       </c>
-      <c r="E107" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="F107" s="9">
-        <f t="shared" si="7"/>
-        <v>86</v>
+      <c r="E107">
+        <v>20</v>
+      </c>
+      <c r="F107" s="8" t="e">
+        <f>+D107*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B108">
         <f>VLOOKUP(C108, 'Base Products'!A:C,2,FALSE)</f>
@@ -3567,17 +3558,17 @@
         <f>VLOOKUP(C108,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E108" s="8">
-        <v>0.1875</v>
-      </c>
-      <c r="F108" s="9">
-        <f t="shared" si="7"/>
-        <v>56.25</v>
+      <c r="E108">
+        <v>18.75</v>
+      </c>
+      <c r="F108" s="8" t="e">
+        <f>+D108*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B109">
         <f>VLOOKUP(C109, 'Base Products'!A:C,2,FALSE)</f>
@@ -3590,17 +3581,17 @@
         <f>VLOOKUP(C109,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E109" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F109" s="9">
-        <f t="shared" si="7"/>
-        <v>30</v>
+      <c r="E109">
+        <v>10</v>
+      </c>
+      <c r="F109" s="8" t="e">
+        <f>+D109*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B110">
         <f>VLOOKUP(C110, 'Base Products'!A:C,2,FALSE)</f>
@@ -3613,17 +3604,17 @@
         <f>VLOOKUP(C110,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>260</v>
       </c>
-      <c r="E110" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F110" s="9">
-        <f t="shared" si="7"/>
-        <v>26</v>
+      <c r="E110">
+        <v>10</v>
+      </c>
+      <c r="F110" s="8" t="e">
+        <f>+D110*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B111">
         <f>VLOOKUP(C111, 'Base Products'!A:C,2,FALSE)</f>
@@ -3636,17 +3627,17 @@
         <f>VLOOKUP(C111,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>315</v>
       </c>
-      <c r="E111" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F111" s="9">
-        <f t="shared" si="7"/>
-        <v>31.5</v>
+      <c r="E111">
+        <v>10</v>
+      </c>
+      <c r="F111" s="8" t="e">
+        <f>+D111*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B112">
         <f>VLOOKUP(C112, 'Base Products'!A:C,2,FALSE)</f>
@@ -3659,17 +3650,17 @@
         <f>VLOOKUP(C112,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>250</v>
       </c>
-      <c r="E112" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="F112" s="9">
-        <f t="shared" si="7"/>
-        <v>12.5</v>
+      <c r="E112">
+        <v>5</v>
+      </c>
+      <c r="F112" s="8" t="e">
+        <f>+D112*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B113">
         <f>VLOOKUP(C113, 'Base Products'!A:C,2,FALSE)</f>
@@ -3682,17 +3673,17 @@
         <f>VLOOKUP(C113,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>53</v>
       </c>
-      <c r="E113" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F113" s="9">
-        <f t="shared" si="7"/>
-        <v>1.06</v>
+      <c r="E113">
+        <v>2</v>
+      </c>
+      <c r="F113" s="8" t="e">
+        <f>+D113*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B114">
         <f>VLOOKUP(C114, 'Base Products'!A:C,2,FALSE)</f>
@@ -3705,17 +3696,17 @@
         <f>VLOOKUP(C114,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>226</v>
       </c>
-      <c r="E114" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F114" s="9">
-        <f t="shared" si="7"/>
-        <v>2.2600000000000002</v>
+      <c r="E114">
+        <v>1</v>
+      </c>
+      <c r="F114" s="8" t="e">
+        <f>+D114*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B115">
         <f>VLOOKUP(C115, 'Base Products'!A:C,2,FALSE)</f>
@@ -3728,17 +3719,17 @@
         <f>VLOOKUP(C115,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>594</v>
       </c>
-      <c r="E115" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F115" s="9">
-        <f t="shared" si="7"/>
-        <v>5.94</v>
+      <c r="E115">
+        <v>1</v>
+      </c>
+      <c r="F115" s="8" t="e">
+        <f>+D115*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B116">
         <f>VLOOKUP(C116, 'Base Products'!A:C,2,FALSE)</f>
@@ -3751,17 +3742,17 @@
         <f>VLOOKUP(C116,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>264</v>
       </c>
-      <c r="E116" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F116" s="9">
-        <f t="shared" si="7"/>
-        <v>2.64</v>
+      <c r="E116">
+        <v>1</v>
+      </c>
+      <c r="F116" s="8" t="e">
+        <f>+D116*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B117">
         <f>VLOOKUP(C117, 'Base Products'!A:C,2,FALSE)</f>
@@ -3774,21 +3765,21 @@
         <f>VLOOKUP(C117,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>575</v>
       </c>
-      <c r="E117" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F117" s="9">
-        <f t="shared" si="7"/>
-        <v>5.75</v>
+      <c r="E117">
+        <v>1</v>
+      </c>
+      <c r="F117" s="8" t="e">
+        <f>+D117*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B118">
         <f>VLOOKUP(C118, 'Base Products'!A:C,2,FALSE)</f>
-        <v>0</v>
+        <v>2040</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>16</v>
@@ -3797,17 +3788,17 @@
         <f>VLOOKUP(C118,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>2701</v>
       </c>
-      <c r="E118" s="8">
-        <v>2E-3</v>
-      </c>
-      <c r="F118" s="9">
-        <f t="shared" si="7"/>
-        <v>5.4020000000000001</v>
+      <c r="E118">
+        <v>0.2</v>
+      </c>
+      <c r="F118" s="8" t="e">
+        <f>+D118*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B119">
         <f>VLOOKUP(C119, 'Base Products'!A:C,2,FALSE)</f>
@@ -3820,17 +3811,17 @@
         <f>VLOOKUP(C119,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>7271</v>
       </c>
-      <c r="E119" s="8">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="F119" s="9">
-        <f t="shared" si="7"/>
-        <v>3.6355</v>
+      <c r="E119">
+        <v>0.05</v>
+      </c>
+      <c r="F119" s="8" t="e">
+        <f>+D119*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B121">
         <f>VLOOKUP(C121, 'Base Products'!A:C,2,FALSE)</f>
@@ -3843,17 +3834,17 @@
         <f>VLOOKUP(C121,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>450</v>
       </c>
-      <c r="E121" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="F121" s="9">
-        <f t="shared" ref="F121:F137" si="8">+D121*E121</f>
-        <v>90</v>
+      <c r="E121">
+        <v>20</v>
+      </c>
+      <c r="F121" s="8" t="e">
+        <f>+D121*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B122">
         <f>VLOOKUP(C122, 'Base Products'!A:C,2,FALSE)</f>
@@ -3866,17 +3857,17 @@
         <f>VLOOKUP(C122,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>430</v>
       </c>
-      <c r="E122" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="F122" s="9">
-        <f t="shared" si="8"/>
-        <v>86</v>
+      <c r="E122">
+        <v>20</v>
+      </c>
+      <c r="F122" s="8" t="e">
+        <f>+D122*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B123">
         <f>VLOOKUP(C123, 'Base Products'!A:C,2,FALSE)</f>
@@ -3889,17 +3880,17 @@
         <f>VLOOKUP(C123,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E123" s="8">
-        <v>0.1663</v>
-      </c>
-      <c r="F123" s="9">
-        <f t="shared" si="8"/>
-        <v>49.89</v>
+      <c r="E123">
+        <v>16.63</v>
+      </c>
+      <c r="F123" s="8" t="e">
+        <f>+D123*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B124">
         <f>VLOOKUP(C124, 'Base Products'!A:C,2,FALSE)</f>
@@ -3912,17 +3903,17 @@
         <f>VLOOKUP(C124,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E124" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F124" s="9">
-        <f t="shared" si="8"/>
-        <v>30</v>
+      <c r="E124">
+        <v>10</v>
+      </c>
+      <c r="F124" s="8" t="e">
+        <f>+D124*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B125">
         <f>VLOOKUP(C125, 'Base Products'!A:C,2,FALSE)</f>
@@ -3935,17 +3926,17 @@
         <f>VLOOKUP(C125,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>260</v>
       </c>
-      <c r="E125" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F125" s="9">
-        <f t="shared" si="8"/>
-        <v>26</v>
+      <c r="E125">
+        <v>10</v>
+      </c>
+      <c r="F125" s="8" t="e">
+        <f>+D125*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B126">
         <f>VLOOKUP(C126, 'Base Products'!A:C,2,FALSE)</f>
@@ -3958,17 +3949,17 @@
         <f>VLOOKUP(C126,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>315</v>
       </c>
-      <c r="E126" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F126" s="9">
-        <f t="shared" si="8"/>
-        <v>31.5</v>
+      <c r="E126">
+        <v>10</v>
+      </c>
+      <c r="F126" s="8" t="e">
+        <f>+D126*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B127">
         <f>VLOOKUP(C127, 'Base Products'!A:C,2,FALSE)</f>
@@ -3981,17 +3972,17 @@
         <f>VLOOKUP(C127,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>250</v>
       </c>
-      <c r="E127" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="F127" s="9">
-        <f t="shared" si="8"/>
-        <v>12.5</v>
+      <c r="E127">
+        <v>5</v>
+      </c>
+      <c r="F127" s="8" t="e">
+        <f>+D127*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B128">
         <f>VLOOKUP(C128, 'Base Products'!A:C,2,FALSE)</f>
@@ -4004,17 +3995,17 @@
         <f>VLOOKUP(C128,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>1000</v>
       </c>
-      <c r="E128" s="8">
-        <v>0.03</v>
-      </c>
-      <c r="F128" s="9">
-        <f t="shared" si="8"/>
-        <v>30</v>
+      <c r="E128">
+        <v>3</v>
+      </c>
+      <c r="F128" s="8" t="e">
+        <f>+D128*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B129">
         <f>VLOOKUP(C129, 'Base Products'!A:C,2,FALSE)</f>
@@ -4027,17 +4018,17 @@
         <f>VLOOKUP(C129,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>53</v>
       </c>
-      <c r="E129" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F129" s="9">
-        <f t="shared" si="8"/>
-        <v>1.06</v>
+      <c r="E129">
+        <v>2</v>
+      </c>
+      <c r="F129" s="8" t="e">
+        <f>+D129*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B130">
         <f>VLOOKUP(C130, 'Base Products'!A:C,2,FALSE)</f>
@@ -4050,17 +4041,17 @@
         <f>VLOOKUP(C130,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>264</v>
       </c>
-      <c r="E130" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F130" s="9">
-        <f t="shared" si="8"/>
-        <v>2.64</v>
+      <c r="E130">
+        <v>1</v>
+      </c>
+      <c r="F130" s="8" t="e">
+        <f>+D130*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B131">
         <f>VLOOKUP(C131, 'Base Products'!A:C,2,FALSE)</f>
@@ -4073,17 +4064,17 @@
         <f>VLOOKUP(C131,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>575</v>
       </c>
-      <c r="E131" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F131" s="9">
-        <f t="shared" si="8"/>
-        <v>5.75</v>
+      <c r="E131">
+        <v>1</v>
+      </c>
+      <c r="F131" s="8" t="e">
+        <f>+D131*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B132">
         <f>VLOOKUP(C132, 'Base Products'!A:C,2,FALSE)</f>
@@ -4096,17 +4087,17 @@
         <f>VLOOKUP(C132,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>594</v>
       </c>
-      <c r="E132" s="8">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F132" s="9">
-        <f t="shared" si="8"/>
-        <v>2.97</v>
+      <c r="E132">
+        <v>0.5</v>
+      </c>
+      <c r="F132" s="8" t="e">
+        <f>+D132*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B133">
         <f>VLOOKUP(C133, 'Base Products'!A:C,2,FALSE)</f>
@@ -4119,21 +4110,21 @@
         <f>VLOOKUP(C133,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>627</v>
       </c>
-      <c r="E133" s="8">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F133" s="9">
-        <f t="shared" si="8"/>
-        <v>3.1350000000000002</v>
+      <c r="E133">
+        <v>0.5</v>
+      </c>
+      <c r="F133" s="8" t="e">
+        <f>+D133*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B134">
         <f>VLOOKUP(C134, 'Base Products'!A:C,2,FALSE)</f>
-        <v>0</v>
+        <v>2040</v>
       </c>
       <c r="C134" s="5" t="s">
         <v>16</v>
@@ -4142,17 +4133,17 @@
         <f>VLOOKUP(C134,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>2701</v>
       </c>
-      <c r="E134" s="8">
-        <v>2E-3</v>
-      </c>
-      <c r="F134" s="9">
-        <f t="shared" si="8"/>
-        <v>5.4020000000000001</v>
+      <c r="E134">
+        <v>0.2</v>
+      </c>
+      <c r="F134" s="8" t="e">
+        <f>+D134*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B135">
         <f>VLOOKUP(C135, 'Base Products'!A:C,2,FALSE)</f>
@@ -4165,17 +4156,17 @@
         <f>VLOOKUP(C135,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>12375</v>
       </c>
-      <c r="E135" s="8">
-        <v>1E-3</v>
-      </c>
-      <c r="F135" s="9">
-        <f t="shared" si="8"/>
-        <v>12.375</v>
+      <c r="E135">
+        <v>0.1</v>
+      </c>
+      <c r="F135" s="8" t="e">
+        <f>+D135*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B136">
         <f>VLOOKUP(C136, 'Base Products'!A:C,2,FALSE)</f>
@@ -4188,17 +4179,17 @@
         <f>VLOOKUP(C136,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>7271</v>
       </c>
-      <c r="E136" s="8">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="F136" s="9">
-        <f t="shared" si="8"/>
-        <v>3.6355</v>
+      <c r="E136">
+        <v>0.05</v>
+      </c>
+      <c r="F136" s="8" t="e">
+        <f>+D136*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B137">
         <f>VLOOKUP(C137, 'Base Products'!A:C,2,FALSE)</f>
@@ -4211,17 +4202,17 @@
         <f>VLOOKUP(C137,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>16550</v>
       </c>
-      <c r="E137" s="8">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="F137" s="9">
-        <f t="shared" si="8"/>
-        <v>3.31</v>
+      <c r="E137">
+        <v>0.02</v>
+      </c>
+      <c r="F137" s="8" t="e">
+        <f>+D137*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B139">
         <f>VLOOKUP(C139, 'Base Products'!A:C,2,FALSE)</f>
@@ -4234,17 +4225,17 @@
         <f>VLOOKUP(C139,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>944</v>
       </c>
-      <c r="E139" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="F139" s="9">
-        <f t="shared" ref="F139:F146" si="9">+D139*E139</f>
-        <v>188.8</v>
+      <c r="E139">
+        <v>20</v>
+      </c>
+      <c r="F139" s="8" t="e">
+        <f>+D139*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B140">
         <f>VLOOKUP(C140, 'Base Products'!A:C,2,FALSE)</f>
@@ -4257,17 +4248,17 @@
         <f>VLOOKUP(C140,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>450</v>
       </c>
-      <c r="E140" s="8">
-        <v>0.17</v>
-      </c>
-      <c r="F140" s="9">
-        <f t="shared" si="9"/>
-        <v>76.5</v>
+      <c r="E140">
+        <v>17</v>
+      </c>
+      <c r="F140" s="8" t="e">
+        <f>+D140*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B141">
         <f>VLOOKUP(C141, 'Base Products'!A:C,2,FALSE)</f>
@@ -4280,17 +4271,17 @@
         <f>VLOOKUP(C141,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>430</v>
       </c>
-      <c r="E141" s="8">
-        <v>0.17</v>
-      </c>
-      <c r="F141" s="9">
-        <f t="shared" si="9"/>
-        <v>73.100000000000009</v>
+      <c r="E141">
+        <v>17</v>
+      </c>
+      <c r="F141" s="8" t="e">
+        <f>+D141*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B142">
         <f>VLOOKUP(C142, 'Base Products'!A:C,2,FALSE)</f>
@@ -4303,17 +4294,17 @@
         <f>VLOOKUP(C142,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E142" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="F142" s="9">
-        <f t="shared" si="9"/>
-        <v>45</v>
+      <c r="E142">
+        <v>15</v>
+      </c>
+      <c r="F142" s="8" t="e">
+        <f>+D142*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B143">
         <f>VLOOKUP(C143, 'Base Products'!A:C,2,FALSE)</f>
@@ -4326,17 +4317,17 @@
         <f>VLOOKUP(C143,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>260</v>
       </c>
-      <c r="E143" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="F143" s="9">
-        <f t="shared" si="9"/>
-        <v>39</v>
+      <c r="E143">
+        <v>15</v>
+      </c>
+      <c r="F143" s="8" t="e">
+        <f>+D143*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B144">
         <f>VLOOKUP(C144, 'Base Products'!A:C,2,FALSE)</f>
@@ -4349,17 +4340,17 @@
         <f>VLOOKUP(C144,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E144" s="8">
-        <v>0.13</v>
-      </c>
-      <c r="F144" s="9">
-        <f t="shared" si="9"/>
-        <v>39</v>
+      <c r="E144">
+        <v>13</v>
+      </c>
+      <c r="F144" s="8" t="e">
+        <f>+D144*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B145">
         <f>VLOOKUP(C145, 'Base Products'!A:C,2,FALSE)</f>
@@ -4372,17 +4363,17 @@
         <f>VLOOKUP(C145,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>970</v>
       </c>
-      <c r="E145" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F145" s="9">
-        <f t="shared" si="9"/>
-        <v>19.400000000000002</v>
+      <c r="E145">
+        <v>2</v>
+      </c>
+      <c r="F145" s="8" t="e">
+        <f>+D145*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B146">
         <f>VLOOKUP(C146, 'Base Products'!A:C,2,FALSE)</f>
@@ -4395,23 +4386,22 @@
         <f>VLOOKUP(C146,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>575</v>
       </c>
-      <c r="E146" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F146" s="9">
-        <f t="shared" si="9"/>
-        <v>5.75</v>
+      <c r="E146">
+        <v>1</v>
+      </c>
+      <c r="F146" s="8" t="e">
+        <f>+D146*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C147" s="5"/>
       <c r="D147" s="5"/>
-      <c r="E147" s="13"/>
-      <c r="F147" s="9"/>
+      <c r="F147" s="8"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B148">
         <f>VLOOKUP(C148, 'Base Products'!A:C,2,FALSE)</f>
@@ -4424,17 +4414,17 @@
         <f>VLOOKUP(C148,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E148" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F148" s="9">
-        <f t="shared" ref="F148:F158" si="10">+D148*E148</f>
-        <v>30</v>
+      <c r="E148">
+        <v>10</v>
+      </c>
+      <c r="F148" s="8" t="e">
+        <f>+D148*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B149">
         <f>VLOOKUP(C149, 'Base Products'!A:C,2,FALSE)</f>
@@ -4447,17 +4437,17 @@
         <f>VLOOKUP(C149,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>285</v>
       </c>
-      <c r="E149" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="F149" s="9">
-        <f t="shared" si="10"/>
-        <v>42.75</v>
+      <c r="E149">
+        <v>15</v>
+      </c>
+      <c r="F149" s="8" t="e">
+        <f>+D149*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B150">
         <f>VLOOKUP(C150, 'Base Products'!A:C,2,FALSE)</f>
@@ -4470,17 +4460,17 @@
         <f>VLOOKUP(C150,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>250</v>
       </c>
-      <c r="E150" s="8">
-        <v>0.24</v>
-      </c>
-      <c r="F150" s="9">
-        <f t="shared" si="10"/>
-        <v>60</v>
+      <c r="E150">
+        <v>24</v>
+      </c>
+      <c r="F150" s="8" t="e">
+        <f>+D150*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B151">
         <f>VLOOKUP(C151, 'Base Products'!A:C,2,FALSE)</f>
@@ -4493,17 +4483,17 @@
         <f>VLOOKUP(C151,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>275</v>
       </c>
-      <c r="E151" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F151" s="9">
-        <f t="shared" si="10"/>
-        <v>27.5</v>
+      <c r="E151">
+        <v>10</v>
+      </c>
+      <c r="F151" s="8" t="e">
+        <f>+D151*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B152">
         <f>VLOOKUP(C152, 'Base Products'!A:C,2,FALSE)</f>
@@ -4516,17 +4506,17 @@
         <f>VLOOKUP(C152,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>101</v>
       </c>
-      <c r="E152" s="8">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F152" s="9">
-        <f t="shared" si="10"/>
-        <v>7.07</v>
+      <c r="E152">
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="F152" s="8" t="e">
+        <f>+D152*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B153">
         <f>VLOOKUP(C153, 'Base Products'!A:C,2,FALSE)</f>
@@ -4539,17 +4529,17 @@
         <f>VLOOKUP(C153,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>220</v>
       </c>
-      <c r="E153" s="8">
-        <v>0.192</v>
-      </c>
-      <c r="F153" s="9">
-        <f t="shared" si="10"/>
-        <v>42.24</v>
+      <c r="E153">
+        <v>19.2</v>
+      </c>
+      <c r="F153" s="8" t="e">
+        <f>+D153*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B154">
         <f>VLOOKUP(C154, 'Base Products'!A:C,2,FALSE)</f>
@@ -4562,17 +4552,17 @@
         <f>VLOOKUP(C154,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>210</v>
       </c>
-      <c r="E154" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F154" s="9">
-        <f t="shared" si="10"/>
-        <v>21</v>
+      <c r="E154">
+        <v>10</v>
+      </c>
+      <c r="F154" s="8" t="e">
+        <f>+D154*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B155">
         <f>VLOOKUP(C155, 'Base Products'!A:C,2,FALSE)</f>
@@ -4585,17 +4575,17 @@
         <f>VLOOKUP(C155,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>53</v>
       </c>
-      <c r="E155" s="8">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F155" s="9">
-        <f t="shared" si="10"/>
-        <v>0.79499999999999993</v>
+      <c r="E155">
+        <v>1.5</v>
+      </c>
+      <c r="F155" s="8" t="e">
+        <f>+D155*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B156">
         <f>VLOOKUP(C156, 'Base Products'!A:C,2,FALSE)</f>
@@ -4608,17 +4598,17 @@
         <f>VLOOKUP(C156,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>970</v>
       </c>
-      <c r="E156" s="8">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F156" s="9">
-        <f t="shared" si="10"/>
-        <v>14.549999999999999</v>
+      <c r="E156">
+        <v>1.5</v>
+      </c>
+      <c r="F156" s="8" t="e">
+        <f>+D156*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B157">
         <f>VLOOKUP(C157, 'Base Products'!A:C,2,FALSE)</f>
@@ -4631,17 +4621,17 @@
         <f>VLOOKUP(C157,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>1113</v>
       </c>
-      <c r="E157" s="8">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="F157" s="9">
-        <f t="shared" si="10"/>
-        <v>8.9039999999999999</v>
+      <c r="E157">
+        <v>0.8</v>
+      </c>
+      <c r="F157" s="8" t="e">
+        <f>+D157*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B158">
         <f>VLOOKUP(C158, 'Base Products'!A:C,2,FALSE)</f>
@@ -4654,17 +4644,17 @@
         <f>VLOOKUP(C158,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>264</v>
       </c>
-      <c r="E158" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="F158" s="9">
-        <f t="shared" si="10"/>
-        <v>2.64</v>
+      <c r="E158">
+        <v>1</v>
+      </c>
+      <c r="F158" s="8" t="e">
+        <f>+D158*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B160">
         <f>VLOOKUP(C160, 'Base Products'!A:C,2,FALSE)</f>
@@ -4677,17 +4667,17 @@
         <f>VLOOKUP(C160,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>250</v>
       </c>
-      <c r="E160" s="8">
-        <v>0.25</v>
-      </c>
-      <c r="F160" s="9">
-        <f t="shared" ref="F160:F166" si="11">+D160*E160</f>
-        <v>62.5</v>
+      <c r="E160">
+        <v>25</v>
+      </c>
+      <c r="F160" s="8" t="e">
+        <f>+D160*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B161">
         <f>VLOOKUP(C161, 'Base Products'!A:C,2,FALSE)</f>
@@ -4700,17 +4690,17 @@
         <f>VLOOKUP(C161,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>101</v>
       </c>
-      <c r="E161" s="8">
+      <c r="E161">
         <v>0</v>
       </c>
-      <c r="F161" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
+      <c r="F161" s="8" t="e">
+        <f>+D161*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B162">
         <f>VLOOKUP(C162, 'Base Products'!A:C,2,FALSE)</f>
@@ -4723,17 +4713,17 @@
         <f>VLOOKUP(C162,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>285</v>
       </c>
-      <c r="E162" s="8">
+      <c r="E162">
         <v>0</v>
       </c>
-      <c r="F162" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
+      <c r="F162" s="8" t="e">
+        <f>+D162*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B163">
         <f>VLOOKUP(C163, 'Base Products'!A:C,2,FALSE)</f>
@@ -4746,17 +4736,17 @@
         <f>VLOOKUP(C163,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E163" s="8">
+      <c r="E163">
         <v>0</v>
       </c>
-      <c r="F163" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
+      <c r="F163" s="8" t="e">
+        <f>+D163*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B164">
         <f>VLOOKUP(C164, 'Base Products'!A:C,2,FALSE)</f>
@@ -4769,17 +4759,17 @@
         <f>VLOOKUP(C164,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>260</v>
       </c>
-      <c r="E164" s="13">
-        <v>0.25</v>
-      </c>
-      <c r="F164" s="9">
-        <f t="shared" si="11"/>
-        <v>65</v>
+      <c r="E164">
+        <v>25</v>
+      </c>
+      <c r="F164" s="8" t="e">
+        <f>+D164*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B165">
         <f>VLOOKUP(C165, 'Base Products'!A:C,2,FALSE)</f>
@@ -4792,17 +4782,17 @@
         <f>VLOOKUP(C165,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>275</v>
       </c>
-      <c r="E165" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="F165" s="9">
-        <f t="shared" si="11"/>
-        <v>55</v>
+      <c r="E165">
+        <v>20</v>
+      </c>
+      <c r="F165" s="8" t="e">
+        <f>+D165*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B166">
         <f>VLOOKUP(C166, 'Base Products'!A:C,2,FALSE)</f>
@@ -4815,23 +4805,22 @@
         <f>VLOOKUP(C166,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>127</v>
       </c>
-      <c r="E166" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="F166" s="9">
-        <f t="shared" si="11"/>
-        <v>38.1</v>
+      <c r="E166">
+        <v>30</v>
+      </c>
+      <c r="F166" s="8" t="e">
+        <f>+D166*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C167" s="5"/>
       <c r="D167" s="5"/>
-      <c r="E167" s="13"/>
-      <c r="F167" s="9"/>
+      <c r="F167" s="8"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B168">
         <f>VLOOKUP(C168, 'Base Products'!A:C,2,FALSE)</f>
@@ -4844,17 +4833,17 @@
         <f>VLOOKUP(C168,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>250</v>
       </c>
-      <c r="E168" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="F168" s="9">
-        <f t="shared" ref="F168:F172" si="12">+D168*E168</f>
-        <v>100</v>
+      <c r="E168">
+        <v>40</v>
+      </c>
+      <c r="F168" s="8" t="e">
+        <f>+D168*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B169">
         <f>VLOOKUP(C169, 'Base Products'!A:C,2,FALSE)</f>
@@ -4867,17 +4856,17 @@
         <f>VLOOKUP(C169,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>101</v>
       </c>
-      <c r="E169" s="8">
-        <v>0.6</v>
-      </c>
-      <c r="F169" s="9">
-        <f t="shared" si="12"/>
-        <v>60.599999999999994</v>
+      <c r="E169">
+        <v>60</v>
+      </c>
+      <c r="F169" s="8" t="e">
+        <f>+D169*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B170">
         <f>VLOOKUP(C170, 'Base Products'!A:C,2,FALSE)</f>
@@ -4890,17 +4879,17 @@
         <f>VLOOKUP(C170,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>285</v>
       </c>
-      <c r="E170" s="8">
+      <c r="E170">
         <v>0</v>
       </c>
-      <c r="F170" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+      <c r="F170" s="8" t="e">
+        <f>+D170*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B171">
         <f>VLOOKUP(C171, 'Base Products'!A:C,2,FALSE)</f>
@@ -4913,17 +4902,17 @@
         <f>VLOOKUP(C171,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E171" s="8">
+      <c r="E171">
         <v>0</v>
       </c>
-      <c r="F171" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+      <c r="F171" s="8" t="e">
+        <f>+D171*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B172">
         <f>VLOOKUP(C172, 'Base Products'!A:C,2,FALSE)</f>
@@ -4936,17 +4925,17 @@
         <f>VLOOKUP(C172,[1]Prices!$A$4:$B$35,2,FALSE)</f>
         <v>260</v>
       </c>
-      <c r="E172" s="13">
+      <c r="E172">
         <v>0</v>
       </c>
-      <c r="F172" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
+      <c r="F172" s="8" t="e">
+        <f>+D172*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B174">
         <f>VLOOKUP(C174, 'Base Products'!A:C,2,FALSE)</f>
@@ -4959,17 +4948,17 @@
         <f>VLOOKUP(C174,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E174" s="12">
-        <v>0.23</v>
-      </c>
-      <c r="F174" s="9">
-        <f t="shared" ref="F174:F181" si="13">+D174*E174</f>
-        <v>69</v>
+      <c r="E174">
+        <v>23</v>
+      </c>
+      <c r="F174" s="8" t="e">
+        <f>+D174*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B175">
         <f>VLOOKUP(C175, 'Base Products'!A:C,2,FALSE)</f>
@@ -4982,17 +4971,17 @@
         <f>VLOOKUP(C175,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>260</v>
       </c>
-      <c r="E175" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="F175" s="9">
-        <f t="shared" si="13"/>
-        <v>52</v>
+      <c r="E175">
+        <v>20</v>
+      </c>
+      <c r="F175" s="8" t="e">
+        <f>+D175*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B176">
         <f>VLOOKUP(C176, 'Base Products'!A:C,2,FALSE)</f>
@@ -5005,40 +4994,40 @@
         <f>VLOOKUP(C176,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>315</v>
       </c>
-      <c r="E176" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="F176" s="9">
-        <f t="shared" si="13"/>
-        <v>31.5</v>
+      <c r="E176">
+        <v>10</v>
+      </c>
+      <c r="F176" s="8" t="e">
+        <f>+D176*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B177">
         <f>VLOOKUP(C177, 'Base Products'!A:C,2,FALSE)</f>
         <v>2028</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D177" s="5">
         <f>VLOOKUP(C177,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>300</v>
       </c>
-      <c r="E177" s="12">
-        <v>0.15</v>
-      </c>
-      <c r="F177" s="9">
-        <f t="shared" si="13"/>
-        <v>45</v>
+      <c r="E177">
+        <v>15</v>
+      </c>
+      <c r="F177" s="8" t="e">
+        <f>+D177*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B178">
         <f>VLOOKUP(C178, 'Base Products'!A:C,2,FALSE)</f>
@@ -5051,17 +5040,17 @@
         <f>VLOOKUP(C178,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>285</v>
       </c>
-      <c r="E178" s="12">
-        <v>0.15</v>
-      </c>
-      <c r="F178" s="9">
-        <f t="shared" si="13"/>
-        <v>42.75</v>
+      <c r="E178">
+        <v>15</v>
+      </c>
+      <c r="F178" s="8" t="e">
+        <f>+D178*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B179">
         <f>VLOOKUP(C179, 'Base Products'!A:C,2,FALSE)</f>
@@ -5074,17 +5063,17 @@
         <f>VLOOKUP(C179,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>101</v>
       </c>
-      <c r="E179" s="12">
-        <v>0.15</v>
-      </c>
-      <c r="F179" s="9">
-        <f t="shared" si="13"/>
-        <v>15.149999999999999</v>
+      <c r="E179">
+        <v>15</v>
+      </c>
+      <c r="F179" s="8" t="e">
+        <f>+D179*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B180">
         <f>VLOOKUP(C180, 'Base Products'!A:C,2,FALSE)</f>
@@ -5097,17 +5086,17 @@
         <f>VLOOKUP(C180,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>53</v>
       </c>
-      <c r="E180" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="F180" s="9">
-        <f t="shared" si="13"/>
-        <v>0.53</v>
+      <c r="E180">
+        <v>1</v>
+      </c>
+      <c r="F180" s="8" t="e">
+        <f>+D180*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B181">
         <f>VLOOKUP(C181, 'Base Products'!A:C,2,FALSE)</f>
@@ -5120,12 +5109,12 @@
         <f>VLOOKUP(C181,[1]Prices!$A$2:$B$35,2,FALSE)</f>
         <v>264</v>
       </c>
-      <c r="E181" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="F181" s="9">
-        <f t="shared" si="13"/>
-        <v>2.64</v>
+      <c r="E181">
+        <v>1</v>
+      </c>
+      <c r="F181" s="8" t="e">
+        <f>+D181*#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>